<commit_message>
records and collects data from a new sheet ev year
</commit_message>
<xml_diff>
--- a/Files/spread.xlsx
+++ b/Files/spread.xlsx
@@ -4,11 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="individual" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Whole" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2021" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2022" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -502,11 +503,11 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6953125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.71484375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="15.15" customWidth="1" style="8" min="2" max="2"/>
     <col width="13.02" customWidth="1" style="8" min="3" max="4"/>
@@ -551,34 +552,100 @@
         </is>
       </c>
       <c r="L1" s="8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" ht="14.65" customHeight="1" s="9">
-      <c r="A2" s="8" t="n"/>
-      <c r="B2" s="12" t="n"/>
-      <c r="D2" s="12" t="n"/>
-      <c r="G2" s="8" t="n"/>
+      <c r="A2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="n">
+        <v>44141</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>500</v>
+      </c>
+      <c r="D2" s="12" t="n">
+        <v>44269</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>53.75</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>128</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>2100</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="9">
-      <c r="A3" s="8" t="n"/>
-      <c r="B3" s="12" t="n"/>
-      <c r="D3" s="12" t="n"/>
-      <c r="G3" s="8" t="n"/>
+      <c r="A3" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="n">
+        <v>44247</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>600</v>
+      </c>
+      <c r="D3" s="12" t="n">
+        <v>44374</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>54</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>127</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>2700</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="9">
-      <c r="A4" s="8" t="n"/>
-      <c r="B4" s="12" t="n"/>
-      <c r="D4" s="13" t="n"/>
+      <c r="A4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="n">
+        <v>44247</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>600</v>
+      </c>
+      <c r="D4" s="13" t="n">
+        <v>44394</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>56</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>149</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>2800</v>
+      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="9">
-      <c r="A5" s="8" t="n"/>
-      <c r="B5" s="12" t="n"/>
+      <c r="A5" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="n">
+        <v>44323</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>500</v>
+      </c>
       <c r="D5" s="13" t="n"/>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="9">
-      <c r="A6" s="8" t="n"/>
-      <c r="B6" s="12" t="n"/>
+      <c r="A6" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="n">
+        <v>44323</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>500</v>
+      </c>
       <c r="D6" s="13" t="n"/>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="9">
@@ -703,13 +770,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.5625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="31.96" customWidth="1" style="8" min="1" max="1"/>
   </cols>
@@ -798,16 +865,16 @@
         <v>0</v>
       </c>
       <c r="F2" s="8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G2" s="8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H2" s="8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2" s="8" t="n">
         <v>0</v>
@@ -841,13 +908,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="8" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G3" s="8" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H3" s="8" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I3" s="8" t="n">
         <v>0</v>
@@ -884,13 +951,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="8" t="n">
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="G4" s="8" t="n">
-        <v>0</v>
+        <v>624</v>
       </c>
       <c r="H4" s="8" t="n">
-        <v>0</v>
+        <v>969</v>
       </c>
       <c r="I4" s="8" t="n">
         <v>0</v>
@@ -957,41 +1024,16 @@
           <t>Average Age (Days)</t>
         </is>
       </c>
-      <c r="B6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8" t="n">
-        <v>0</v>
-      </c>
       <c r="F6" s="8" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8" t="n">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="H6" s="15" t="inlineStr">
+        <is>
+          <t>94.33</t>
+        </is>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="9">
@@ -1000,42 +1042,345 @@
           <t>Feed per Pig (Kg/pig)</t>
         </is>
       </c>
-      <c r="B7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8" t="n">
-        <v>0</v>
-      </c>
       <c r="F7" s="8" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8" t="n">
-        <v>0</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="9">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>Feed per Age per Pig (Kg/[Day/Pig])</t>
+        </is>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>4.68755</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>2.5974025974026</v>
+      </c>
+      <c r="H8" s="8" t="n"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="37.51" customWidth="1" style="8" min="1" max="1"/>
+    <col width="13.12" customWidth="1" style="8" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.8" customHeight="1" s="9">
+      <c r="A1" s="14" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>January</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="G1" s="8" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="H1" s="8" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="I1" s="8" t="inlineStr">
+        <is>
+          <t>August</t>
+        </is>
+      </c>
+      <c r="J1" s="8" t="inlineStr">
+        <is>
+          <t>September</t>
+        </is>
+      </c>
+      <c r="K1" s="8" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="L1" s="8" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+      <c r="M1" s="8" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="9">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>Population</t>
+        </is>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="9">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>Feed Mass (Kg)</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="9">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>Feed Price (E)</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="9">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>Misc (E)</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="9">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>Average Age (Days)</t>
+        </is>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="12.8" customHeight="1" s="9">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>Feed per Pig (Kg/pig)</t>
+        </is>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="12.8" customHeight="1" s="9">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>Feed per Age per Pig (Kg/[Day/Pig])</t>
+        </is>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
Introduced DataFrames and switched toPlotly
</commit_message>
<xml_diff>
--- a/Files/spread.xlsx
+++ b/Files/spread.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="individual" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2021" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2022" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="individual" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -18,9 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="[hh]:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -85,7 +86,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -127,6 +128,9 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -501,16 +505,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.73046875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.84765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="15.15" customWidth="1" style="8" min="2" max="2"/>
-    <col width="13.02" customWidth="1" style="8" min="3" max="4"/>
+    <col width="15.42" customWidth="1" style="8" min="3" max="3"/>
+    <col width="13.02" customWidth="1" style="8" min="4" max="4"/>
     <col width="14.69" customWidth="1" style="8" min="5" max="5"/>
     <col width="13.43" customWidth="1" style="8" min="6" max="6"/>
   </cols>
@@ -523,37 +528,38 @@
       </c>
       <c r="B1" s="10" t="inlineStr">
         <is>
-          <t>Birth Date</t>
+          <t>birth_date</t>
         </is>
       </c>
       <c r="C1" s="10" t="inlineStr">
         <is>
-          <t>Purchase Price</t>
+          <t>purchase_price</t>
         </is>
       </c>
       <c r="D1" s="11" t="inlineStr">
         <is>
-          <t>Slaughter Date</t>
+          <t>slaughter_date</t>
         </is>
       </c>
       <c r="E1" s="10" t="inlineStr">
         <is>
-          <t>Slaughter Weight</t>
+          <t>slaughter_weight</t>
         </is>
       </c>
       <c r="F1" s="10" t="inlineStr">
         <is>
-          <t>Slaughter Age</t>
+          <t>slaughter_age</t>
         </is>
       </c>
       <c r="G1" s="10" t="inlineStr">
         <is>
-          <t>Sale Price</t>
-        </is>
-      </c>
-      <c r="L1" s="8" t="n">
+          <t>sale_price</t>
+        </is>
+      </c>
+      <c r="H1" s="8" t="n">
         <v>9</v>
       </c>
+      <c r="L1" s="8" t="n"/>
     </row>
     <row r="2" ht="14.65" customHeight="1" s="9">
       <c r="A2" s="8" t="n">
@@ -611,7 +617,7 @@
       <c r="C4" s="8" t="n">
         <v>600</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="12" t="n">
         <v>44394</v>
       </c>
       <c r="E4" s="8" t="n">
@@ -700,10 +706,7 @@
       <c r="B11" s="12" t="n"/>
       <c r="D11" s="13" t="n"/>
     </row>
-    <row r="12" ht="12.75" customHeight="1" s="9">
-      <c r="B12" s="12" t="n"/>
-      <c r="D12" s="13" t="n"/>
-    </row>
+    <row r="12" ht="12.75" customHeight="1" s="9"/>
     <row r="13" ht="12.75" customHeight="1" s="9"/>
     <row r="14" ht="12.75" customHeight="1" s="9"/>
     <row r="15" ht="12.75" customHeight="1" s="9"/>
@@ -780,7 +783,7 @@
     <row r="86" ht="12.75" customHeight="1" s="9"/>
     <row r="87" ht="12.75" customHeight="1" s="9"/>
     <row r="88" ht="12.75" customHeight="1" s="9"/>
-    <row r="89" ht="12.75" customHeight="1" s="9"/>
+    <row r="1048576" ht="12.8" customHeight="1" s="9"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -802,86 +805,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="31.96" customWidth="1" style="8" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="9">
-      <c r="A1" s="14" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B1" s="8" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-      <c r="C1" s="8" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="D1" s="8" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-      <c r="E1" s="8" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-      <c r="F1" s="8" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-      <c r="G1" s="8" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="H1" s="8" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="I1" s="8" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-      <c r="J1" s="8" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="K1" s="8" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-      <c r="L1" s="8" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-      <c r="M1" s="8" t="inlineStr">
-        <is>
-          <t>December</t>
+      <c r="A1" s="14" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>population</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>feed_mass</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>feed_price</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>misc</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>average_age</t>
         </is>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="9">
       <c r="A2" s="8" t="inlineStr">
         <is>
-          <t>Population</t>
+          <t>jan</t>
         </is>
       </c>
       <c r="B2" s="8" t="n">
@@ -897,34 +867,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="I2" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="J2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="9">
       <c r="A3" s="8" t="inlineStr">
         <is>
-          <t>Feed Mass (Kg)</t>
+          <t>feb</t>
         </is>
       </c>
       <c r="B3" s="8" t="n">
@@ -940,34 +889,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="8" t="n">
-        <v>150</v>
-      </c>
-      <c r="G3" s="8" t="n">
-        <v>100</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>200</v>
-      </c>
-      <c r="I3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="9">
       <c r="A4" s="8" t="inlineStr">
         <is>
-          <t>Feed Price (E)</t>
+          <t>mar</t>
         </is>
       </c>
       <c r="B4" s="8" t="n">
@@ -983,34 +911,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="8" t="n">
-        <v>960</v>
-      </c>
-      <c r="G4" s="8" t="n">
-        <v>624</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>1292</v>
-      </c>
-      <c r="I4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="9">
       <c r="A5" s="8" t="inlineStr">
         <is>
-          <t>Misc (E)</t>
+          <t>apr</t>
         </is>
       </c>
       <c r="B5" s="8" t="n">
@@ -1026,77 +933,180 @@
         <v>0</v>
       </c>
       <c r="F5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="9">
       <c r="A6" s="8" t="inlineStr">
         <is>
-          <t>Average Age (Days)</t>
-        </is>
+          <t>may</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>150</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>960</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="F6" s="8" t="n">
         <v>96</v>
       </c>
-      <c r="G6" s="8" t="n">
-        <v>77</v>
-      </c>
-      <c r="H6" s="15" t="inlineStr">
-        <is>
-          <t>94.33</t>
-        </is>
-      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="9">
       <c r="A7" s="8" t="inlineStr">
         <is>
-          <t>Feed per Pig (Kg/pig)</t>
-        </is>
+          <t>jun</t>
+        </is>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>624</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>25</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>33.33333333333334</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="G7" s="8" t="n"/>
+      <c r="H7" s="8" t="n"/>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="9">
       <c r="A8" s="8" t="inlineStr">
         <is>
-          <t>Feed per Age per Pig (Kg/[Day/Pig])</t>
-        </is>
-      </c>
-      <c r="F8" s="8" t="n">
-        <v>4.68755</v>
-      </c>
-      <c r="G8" s="8" t="n">
-        <v>2.5974025974026</v>
-      </c>
+          <t>jul</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>200</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>1292</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="15" t="n">
+        <v>54.81142190972222</v>
+      </c>
+      <c r="G8" s="8" t="n"/>
       <c r="H8" s="8" t="n"/>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>aug</t>
+        </is>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="15" t="n">
+        <v>54.81201430233796</v>
+      </c>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="9">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>sep</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8" t="n"/>
+    </row>
+    <row r="11" ht="12.8" customHeight="1" s="9">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>oct</t>
+        </is>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8" t="n"/>
+    </row>
+    <row r="12" ht="12.8" customHeight="1" s="9">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>nov</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="n"/>
+    </row>
+    <row r="13" ht="12.8" customHeight="1" s="9">
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>dec</t>
+        </is>
+      </c>
+      <c r="B13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1122,10 +1132,10 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="37.51" customWidth="1" style="8" min="1" max="1"/>
     <col width="13.12" customWidth="1" style="8" min="2" max="2"/>
@@ -1380,7 +1390,7 @@
       <c r="G6" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="15" t="n">
+      <c r="H6" s="16" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reverted to matplotlib due to plotly slowing start
</commit_message>
<xml_diff>
--- a/Files/spread.xlsx
+++ b/Files/spread.xlsx
@@ -511,7 +511,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.84765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.84765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="15.15" customWidth="1" style="8" min="2" max="2"/>
     <col width="15.42" customWidth="1" style="8" min="3" max="3"/>
@@ -811,7 +811,7 @@
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="31.96" customWidth="1" style="8" min="1" max="1"/>
   </cols>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>54.81201430233796</v>
+        <v>54.81201430555556</v>
       </c>
     </row>
     <row r="10" ht="12.8" customHeight="1" s="9">
@@ -1135,7 +1135,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="37.51" customWidth="1" style="8" min="1" max="1"/>
     <col width="13.12" customWidth="1" style="8" min="2" max="2"/>

</xml_diff>

<commit_message>
introduced breed type and amount of meds taken
</commit_message>
<xml_diff>
--- a/Files/spread.xlsx
+++ b/Files/spread.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="individual" sheetId="1" state="visible" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -106,6 +106,9 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -505,285 +508,364 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.84765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.921875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="15.15" customWidth="1" style="8" min="2" max="2"/>
-    <col width="15.42" customWidth="1" style="8" min="3" max="3"/>
-    <col width="13.02" customWidth="1" style="8" min="4" max="4"/>
-    <col width="14.69" customWidth="1" style="8" min="5" max="5"/>
-    <col width="13.43" customWidth="1" style="8" min="6" max="6"/>
+    <col width="15.15" customWidth="1" style="9" min="2" max="2"/>
+    <col width="15.42" customWidth="1" style="9" min="3" max="3"/>
+    <col width="13.02" customWidth="1" style="9" min="4" max="4"/>
+    <col width="14.69" customWidth="1" style="9" min="5" max="5"/>
+    <col width="13.43" customWidth="1" style="9" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32.8" customHeight="1" s="9">
-      <c r="A1" s="10" t="inlineStr">
+    <row r="1" ht="32.8" customHeight="1" s="10">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>birth_date</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>purchase_price</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>slaughter_date</t>
         </is>
       </c>
-      <c r="E1" s="10" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>slaughter_weight</t>
         </is>
       </c>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>slaughter_age</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>sale_price</t>
         </is>
       </c>
-      <c r="H1" s="8" t="n">
+      <c r="H1" s="11" t="inlineStr">
+        <is>
+          <t>breed</t>
+        </is>
+      </c>
+      <c r="I1" s="11" t="inlineStr">
+        <is>
+          <t>meds</t>
+        </is>
+      </c>
+      <c r="J1" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="L1" s="8" t="n"/>
-    </row>
-    <row r="2" ht="14.65" customHeight="1" s="9">
-      <c r="A2" s="8" t="n">
+      <c r="L1" s="9" t="n"/>
+    </row>
+    <row r="2" ht="14.65" customHeight="1" s="10">
+      <c r="A2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="n">
+      <c r="B2" s="13" t="n">
         <v>44141</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="13" t="n">
         <v>44269</v>
       </c>
-      <c r="E2" s="8" t="n">
+      <c r="E2" s="9" t="n">
         <v>53.75</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="9" t="n">
         <v>128</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="9" t="n">
         <v>2100</v>
       </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1" s="9">
-      <c r="A3" s="8" t="n">
+      <c r="H2" s="9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="I2" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="10">
+      <c r="A3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="n">
+      <c r="B3" s="13" t="n">
         <v>44247</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="9" t="n">
         <v>600</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="13" t="n">
         <v>44374</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="9" t="n">
         <v>54</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="9" t="n">
         <v>127</v>
       </c>
-      <c r="G3" s="8" t="n">
+      <c r="G3" s="9" t="n">
         <v>2700</v>
       </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="9">
-      <c r="A4" s="8" t="n">
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I3" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="10">
+      <c r="A4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="13" t="n">
         <v>44247</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="9" t="n">
         <v>600</v>
       </c>
-      <c r="D4" s="12" t="n">
+      <c r="D4" s="13" t="n">
         <v>44394</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="9" t="n">
         <v>56</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="9" t="n">
         <v>149</v>
       </c>
-      <c r="G4" s="8" t="n">
+      <c r="G4" s="9" t="n">
         <v>2800</v>
       </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1" s="9">
-      <c r="A5" s="8" t="n">
+      <c r="H4" s="9" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I4" s="9" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1" s="10">
+      <c r="A5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="13" t="n">
         <v>44323</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="D5" s="13" t="n"/>
-    </row>
-    <row r="6" ht="12.75" customHeight="1" s="9">
-      <c r="A6" s="8" t="n">
+      <c r="D5" s="14" t="n"/>
+      <c r="H5" s="9" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="I5" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="10">
+      <c r="A6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="n">
+      <c r="B6" s="13" t="n">
         <v>44323</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="D6" s="13" t="n"/>
-    </row>
-    <row r="7" ht="12.75" customHeight="1" s="9">
-      <c r="A7" s="8" t="n">
+      <c r="D6" s="14" t="n"/>
+      <c r="H6" s="9" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="I6" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="10">
+      <c r="A7" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="13" t="n">
         <v>44368</v>
       </c>
-      <c r="C7" s="8" t="n">
+      <c r="C7" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="D7" s="13" t="n"/>
-    </row>
-    <row r="8" ht="12.75" customHeight="1" s="9">
-      <c r="A8" s="8" t="n">
+      <c r="D7" s="14" t="n"/>
+      <c r="H7" s="9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="I7" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="10">
+      <c r="A8" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="13" t="n">
         <v>44368</v>
       </c>
-      <c r="C8" s="8" t="n">
+      <c r="C8" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="D8" s="13" t="n"/>
-    </row>
-    <row r="9" ht="12.75" customHeight="1" s="9">
-      <c r="A9" s="8" t="n">
+      <c r="D8" s="14" t="n"/>
+      <c r="H8" s="9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="10">
+      <c r="A9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="13" t="n">
         <v>44368</v>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C9" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="D9" s="13" t="n"/>
-    </row>
-    <row r="10" ht="12.75" customHeight="1" s="9">
-      <c r="A10" s="8" t="n">
+      <c r="D9" s="14" t="n"/>
+      <c r="H9" s="9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="I9" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1" s="10">
+      <c r="A10" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="n">
+      <c r="B10" s="13" t="n">
         <v>44368</v>
       </c>
-      <c r="C10" s="8" t="n">
+      <c r="C10" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="D10" s="13" t="n"/>
-    </row>
-    <row r="11" ht="12.75" customHeight="1" s="9">
-      <c r="B11" s="12" t="n"/>
-      <c r="D11" s="13" t="n"/>
-    </row>
-    <row r="12" ht="12.75" customHeight="1" s="9"/>
-    <row r="13" ht="12.75" customHeight="1" s="9"/>
-    <row r="14" ht="12.75" customHeight="1" s="9"/>
-    <row r="15" ht="12.75" customHeight="1" s="9"/>
-    <row r="16" ht="12.75" customHeight="1" s="9"/>
-    <row r="17" ht="12.75" customHeight="1" s="9"/>
-    <row r="18" ht="12.75" customHeight="1" s="9"/>
-    <row r="19" ht="12.75" customHeight="1" s="9"/>
-    <row r="20" ht="12.75" customHeight="1" s="9"/>
-    <row r="21" ht="12.75" customHeight="1" s="9"/>
-    <row r="22" ht="12.75" customHeight="1" s="9"/>
-    <row r="23" ht="12.75" customHeight="1" s="9"/>
-    <row r="24" ht="12.75" customHeight="1" s="9"/>
-    <row r="25" ht="12.75" customHeight="1" s="9"/>
-    <row r="26" ht="12.75" customHeight="1" s="9"/>
-    <row r="27" ht="12.75" customHeight="1" s="9"/>
-    <row r="28" ht="12.75" customHeight="1" s="9"/>
-    <row r="29" ht="12.75" customHeight="1" s="9"/>
-    <row r="30" ht="12.75" customHeight="1" s="9"/>
-    <row r="31" ht="12.75" customHeight="1" s="9"/>
-    <row r="32" ht="12.75" customHeight="1" s="9"/>
-    <row r="33" ht="12.75" customHeight="1" s="9"/>
-    <row r="34" ht="12.75" customHeight="1" s="9"/>
-    <row r="35" ht="12.75" customHeight="1" s="9"/>
-    <row r="36" ht="12.75" customHeight="1" s="9"/>
-    <row r="37" ht="12.75" customHeight="1" s="9"/>
-    <row r="38" ht="12.75" customHeight="1" s="9"/>
-    <row r="39" ht="12.75" customHeight="1" s="9"/>
-    <row r="40" ht="12.75" customHeight="1" s="9"/>
-    <row r="41" ht="12.75" customHeight="1" s="9"/>
-    <row r="42" ht="12.75" customHeight="1" s="9"/>
-    <row r="43" ht="12.75" customHeight="1" s="9"/>
-    <row r="44" ht="12.75" customHeight="1" s="9"/>
-    <row r="45" ht="12.75" customHeight="1" s="9"/>
-    <row r="46" ht="12.75" customHeight="1" s="9"/>
-    <row r="47" ht="12.75" customHeight="1" s="9"/>
-    <row r="48" ht="12.75" customHeight="1" s="9"/>
-    <row r="49" ht="12.75" customHeight="1" s="9"/>
-    <row r="50" ht="12.75" customHeight="1" s="9"/>
-    <row r="51" ht="12.75" customHeight="1" s="9"/>
-    <row r="52" ht="12.75" customHeight="1" s="9"/>
-    <row r="53" ht="12.75" customHeight="1" s="9"/>
-    <row r="54" ht="12.75" customHeight="1" s="9"/>
-    <row r="55" ht="12.75" customHeight="1" s="9"/>
-    <row r="56" ht="12.75" customHeight="1" s="9"/>
-    <row r="57" ht="12.75" customHeight="1" s="9"/>
-    <row r="58" ht="12.75" customHeight="1" s="9"/>
-    <row r="59" ht="12.75" customHeight="1" s="9"/>
-    <row r="60" ht="12.75" customHeight="1" s="9"/>
-    <row r="61" ht="12.75" customHeight="1" s="9"/>
-    <row r="62" ht="12.75" customHeight="1" s="9"/>
-    <row r="63" ht="12.75" customHeight="1" s="9"/>
-    <row r="64" ht="12.75" customHeight="1" s="9"/>
-    <row r="65" ht="12.75" customHeight="1" s="9"/>
-    <row r="66" ht="12.75" customHeight="1" s="9"/>
-    <row r="67" ht="12.75" customHeight="1" s="9"/>
-    <row r="68" ht="12.75" customHeight="1" s="9"/>
-    <row r="69" ht="12.75" customHeight="1" s="9"/>
-    <row r="70" ht="12.75" customHeight="1" s="9"/>
-    <row r="71" ht="12.75" customHeight="1" s="9"/>
-    <row r="72" ht="12.75" customHeight="1" s="9"/>
-    <row r="73" ht="12.75" customHeight="1" s="9"/>
-    <row r="74" ht="12.75" customHeight="1" s="9"/>
-    <row r="75" ht="12.75" customHeight="1" s="9"/>
-    <row r="76" ht="12.75" customHeight="1" s="9"/>
-    <row r="77" ht="12.75" customHeight="1" s="9"/>
-    <row r="78" ht="12.75" customHeight="1" s="9"/>
-    <row r="79" ht="12.75" customHeight="1" s="9"/>
-    <row r="80" ht="12.75" customHeight="1" s="9"/>
-    <row r="81" ht="12.75" customHeight="1" s="9"/>
-    <row r="82" ht="12.75" customHeight="1" s="9"/>
-    <row r="83" ht="12.75" customHeight="1" s="9"/>
-    <row r="84" ht="12.75" customHeight="1" s="9"/>
-    <row r="85" ht="12.75" customHeight="1" s="9"/>
-    <row r="86" ht="12.75" customHeight="1" s="9"/>
-    <row r="87" ht="12.75" customHeight="1" s="9"/>
-    <row r="88" ht="12.75" customHeight="1" s="9"/>
-    <row r="1048576" ht="12.8" customHeight="1" s="9"/>
+      <c r="D10" s="14" t="n"/>
+      <c r="H10" s="9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="I10" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1" s="10"/>
+    <row r="12" ht="12.75" customHeight="1" s="10"/>
+    <row r="13" ht="12.75" customHeight="1" s="10"/>
+    <row r="14" ht="12.75" customHeight="1" s="10"/>
+    <row r="15" ht="12.75" customHeight="1" s="10"/>
+    <row r="16" ht="12.75" customHeight="1" s="10"/>
+    <row r="17" ht="12.75" customHeight="1" s="10"/>
+    <row r="18" ht="12.75" customHeight="1" s="10"/>
+    <row r="19" ht="12.75" customHeight="1" s="10"/>
+    <row r="20" ht="12.75" customHeight="1" s="10"/>
+    <row r="21" ht="12.75" customHeight="1" s="10"/>
+    <row r="22" ht="12.75" customHeight="1" s="10"/>
+    <row r="23" ht="12.75" customHeight="1" s="10"/>
+    <row r="24" ht="12.75" customHeight="1" s="10"/>
+    <row r="25" ht="12.75" customHeight="1" s="10"/>
+    <row r="26" ht="12.75" customHeight="1" s="10"/>
+    <row r="27" ht="12.75" customHeight="1" s="10"/>
+    <row r="28" ht="12.75" customHeight="1" s="10"/>
+    <row r="29" ht="12.75" customHeight="1" s="10"/>
+    <row r="30" ht="12.75" customHeight="1" s="10"/>
+    <row r="31" ht="12.75" customHeight="1" s="10"/>
+    <row r="32" ht="12.75" customHeight="1" s="10"/>
+    <row r="33" ht="12.75" customHeight="1" s="10"/>
+    <row r="34" ht="12.75" customHeight="1" s="10"/>
+    <row r="35" ht="12.75" customHeight="1" s="10"/>
+    <row r="36" ht="12.75" customHeight="1" s="10"/>
+    <row r="37" ht="12.75" customHeight="1" s="10"/>
+    <row r="38" ht="12.75" customHeight="1" s="10"/>
+    <row r="39" ht="12.75" customHeight="1" s="10"/>
+    <row r="40" ht="12.75" customHeight="1" s="10"/>
+    <row r="41" ht="12.75" customHeight="1" s="10"/>
+    <row r="42" ht="12.75" customHeight="1" s="10"/>
+    <row r="43" ht="12.75" customHeight="1" s="10"/>
+    <row r="44" ht="12.75" customHeight="1" s="10"/>
+    <row r="45" ht="12.75" customHeight="1" s="10"/>
+    <row r="46" ht="12.75" customHeight="1" s="10"/>
+    <row r="47" ht="12.75" customHeight="1" s="10"/>
+    <row r="48" ht="12.75" customHeight="1" s="10"/>
+    <row r="49" ht="12.75" customHeight="1" s="10"/>
+    <row r="50" ht="12.75" customHeight="1" s="10"/>
+    <row r="51" ht="12.75" customHeight="1" s="10"/>
+    <row r="52" ht="12.75" customHeight="1" s="10"/>
+    <row r="53" ht="12.75" customHeight="1" s="10"/>
+    <row r="54" ht="12.75" customHeight="1" s="10"/>
+    <row r="55" ht="12.75" customHeight="1" s="10"/>
+    <row r="56" ht="12.75" customHeight="1" s="10"/>
+    <row r="57" ht="12.75" customHeight="1" s="10"/>
+    <row r="58" ht="12.75" customHeight="1" s="10"/>
+    <row r="59" ht="12.75" customHeight="1" s="10"/>
+    <row r="60" ht="12.75" customHeight="1" s="10"/>
+    <row r="61" ht="12.75" customHeight="1" s="10"/>
+    <row r="62" ht="12.75" customHeight="1" s="10"/>
+    <row r="63" ht="12.75" customHeight="1" s="10"/>
+    <row r="64" ht="12.75" customHeight="1" s="10"/>
+    <row r="65" ht="12.75" customHeight="1" s="10"/>
+    <row r="66" ht="12.75" customHeight="1" s="10"/>
+    <row r="67" ht="12.75" customHeight="1" s="10"/>
+    <row r="68" ht="12.75" customHeight="1" s="10"/>
+    <row r="69" ht="12.75" customHeight="1" s="10"/>
+    <row r="70" ht="12.75" customHeight="1" s="10"/>
+    <row r="71" ht="12.75" customHeight="1" s="10"/>
+    <row r="72" ht="12.75" customHeight="1" s="10"/>
+    <row r="73" ht="12.75" customHeight="1" s="10"/>
+    <row r="74" ht="12.75" customHeight="1" s="10"/>
+    <row r="75" ht="12.75" customHeight="1" s="10"/>
+    <row r="76" ht="12.75" customHeight="1" s="10"/>
+    <row r="77" ht="12.75" customHeight="1" s="10"/>
+    <row r="78" ht="12.75" customHeight="1" s="10"/>
+    <row r="79" ht="12.75" customHeight="1" s="10"/>
+    <row r="80" ht="12.75" customHeight="1" s="10"/>
+    <row r="81" ht="12.75" customHeight="1" s="10"/>
+    <row r="82" ht="12.75" customHeight="1" s="10"/>
+    <row r="83" ht="12.75" customHeight="1" s="10"/>
+    <row r="84" ht="12.75" customHeight="1" s="10"/>
+    <row r="85" ht="12.75" customHeight="1" s="10"/>
+    <row r="86" ht="12.75" customHeight="1" s="10"/>
+    <row r="1048574" ht="12.8" customHeight="1" s="10"/>
+    <row r="1048575" ht="12.8" customHeight="1" s="10"/>
+    <row r="1048576" ht="12.8" customHeight="1" s="10"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -807,306 +889,306 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="31.96" customWidth="1" style="8" min="1" max="1"/>
+    <col width="31.96" customWidth="1" style="9" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="9">
-      <c r="A1" s="14" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="10">
+      <c r="A1" s="15" t="inlineStr">
         <is>
           <t>month</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>population</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>feed_mass</t>
         </is>
       </c>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="D1" s="11" t="inlineStr">
         <is>
           <t>feed_price</t>
         </is>
       </c>
-      <c r="E1" s="10" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>misc</t>
         </is>
       </c>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>average_age</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="9">
-      <c r="A2" s="8" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="10">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>jan</t>
         </is>
       </c>
-      <c r="B2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1" s="9">
-      <c r="A3" s="8" t="inlineStr">
+      <c r="B2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="10">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>feb</t>
         </is>
       </c>
-      <c r="B3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="9">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="B3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="10">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>mar</t>
         </is>
       </c>
-      <c r="B4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1" s="9">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="B4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1" s="10">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>apr</t>
         </is>
       </c>
-      <c r="B5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1" s="9">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="B5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="10">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>may</t>
         </is>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="9" t="n">
         <v>150</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="9" t="n">
         <v>960</v>
       </c>
-      <c r="E6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="n">
+      <c r="E6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="n">
         <v>96</v>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1" s="9">
-      <c r="A7" s="8" t="inlineStr">
+    <row r="7" ht="12.75" customHeight="1" s="10">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>jun</t>
         </is>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="n">
+      <c r="C7" s="9" t="n">
         <v>100</v>
       </c>
-      <c r="D7" s="8" t="n">
+      <c r="D7" s="9" t="n">
         <v>624</v>
       </c>
-      <c r="E7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="n">
+      <c r="E7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9" t="n">
         <v>77</v>
       </c>
-      <c r="G7" s="8" t="n"/>
-      <c r="H7" s="8" t="n"/>
-    </row>
-    <row r="8" ht="12.75" customHeight="1" s="9">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="G7" s="9" t="n"/>
+      <c r="H7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="10">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>jul</t>
         </is>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="8" t="n">
+      <c r="C8" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="D8" s="8" t="n">
+      <c r="D8" s="9" t="n">
         <v>1292</v>
       </c>
-      <c r="E8" s="8" t="n">
+      <c r="E8" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="15" t="n">
+      <c r="F8" s="16" t="n">
         <v>54.81142190972222</v>
       </c>
-      <c r="G8" s="8" t="n"/>
-      <c r="H8" s="8" t="n"/>
-    </row>
-    <row r="9" ht="12.8" customHeight="1" s="9">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="G8" s="9" t="n"/>
+      <c r="H8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="10">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>aug</t>
         </is>
       </c>
-      <c r="B9" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="15" t="n">
+      <c r="B9" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16" t="n">
         <v>54.81201430555556</v>
       </c>
     </row>
-    <row r="10" ht="12.8" customHeight="1" s="9">
-      <c r="A10" s="8" t="inlineStr">
+    <row r="10" ht="12.8" customHeight="1" s="10">
+      <c r="A10" s="9" t="inlineStr">
         <is>
           <t>sep</t>
         </is>
       </c>
-      <c r="B10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="n"/>
-    </row>
-    <row r="11" ht="12.8" customHeight="1" s="9">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="B10" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="12.8" customHeight="1" s="10">
+      <c r="A11" s="9" t="inlineStr">
         <is>
           <t>oct</t>
         </is>
       </c>
-      <c r="B11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8" t="n"/>
-    </row>
-    <row r="12" ht="12.8" customHeight="1" s="9">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="B11" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="12.8" customHeight="1" s="10">
+      <c r="A12" s="9" t="inlineStr">
         <is>
           <t>nov</t>
         </is>
       </c>
-      <c r="B12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8" t="n"/>
-    </row>
-    <row r="13" ht="12.8" customHeight="1" s="9">
-      <c r="A13" s="8" t="inlineStr">
+      <c r="B12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9" t="n"/>
+    </row>
+    <row r="13" ht="12.8" customHeight="1" s="10">
+      <c r="A13" s="9" t="inlineStr">
         <is>
           <t>dec</t>
         </is>
       </c>
-      <c r="B13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8" t="n"/>
+      <c r="B13" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1135,294 +1217,294 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="37.51" customWidth="1" style="8" min="1" max="1"/>
-    <col width="13.12" customWidth="1" style="8" min="2" max="2"/>
+    <col width="37.51" customWidth="1" style="9" min="1" max="1"/>
+    <col width="13.12" customWidth="1" style="9" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="9">
-      <c r="A1" s="14" t="n">
+    <row r="1" ht="12.8" customHeight="1" s="10">
+      <c r="A1" s="15" t="n">
         <v>2021</v>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>January</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>February</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>March</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>April</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="9" t="inlineStr">
         <is>
           <t>May</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="9" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>July</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>August</t>
         </is>
       </c>
-      <c r="J1" s="8" t="inlineStr">
+      <c r="J1" s="9" t="inlineStr">
         <is>
           <t>September</t>
         </is>
       </c>
-      <c r="K1" s="8" t="inlineStr">
+      <c r="K1" s="9" t="inlineStr">
         <is>
           <t>October</t>
         </is>
       </c>
-      <c r="L1" s="8" t="inlineStr">
+      <c r="L1" s="9" t="inlineStr">
         <is>
           <t>November</t>
         </is>
       </c>
-      <c r="M1" s="8" t="inlineStr">
+      <c r="M1" s="9" t="inlineStr">
         <is>
           <t>December</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="9">
-      <c r="A2" s="8" t="inlineStr">
+    <row r="2" ht="12.8" customHeight="1" s="10">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Population</t>
         </is>
       </c>
-      <c r="B2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" ht="12.8" customHeight="1" s="9">
-      <c r="A3" s="8" t="inlineStr">
+      <c r="B2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="10">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>Feed Mass (Kg)</t>
         </is>
       </c>
-      <c r="B3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" ht="12.8" customHeight="1" s="9">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="B3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="10">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>Feed Price (E)</t>
         </is>
       </c>
-      <c r="B4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" ht="12.8" customHeight="1" s="9">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="B4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="10">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>Misc (E)</t>
         </is>
       </c>
-      <c r="B5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="12.8" customHeight="1" s="9">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="B5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="10">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>Average Age (Days)</t>
         </is>
       </c>
-      <c r="F6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="12.8" customHeight="1" s="9">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="F6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="12.8" customHeight="1" s="10">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>Feed per Pig (Kg/pig)</t>
         </is>
       </c>
-      <c r="F7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="12.8" customHeight="1" s="9">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="F7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="12.8" customHeight="1" s="10">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>Feed per Age per Pig (Kg/[Day/Pig])</t>
         </is>
       </c>
-      <c r="F8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="8" t="n"/>
+      <c r="F8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
added an estimate mass for feed eaten by each pig
</commit_message>
<xml_diff>
--- a/Files/spread.xlsx
+++ b/Files/spread.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -51,6 +51,12 @@
     <t xml:space="preserve">meds</t>
   </si>
   <si>
+    <t xml:space="preserve">feed_eaten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purchase_date</t>
+  </si>
+  <si>
     <t xml:space="preserve">n</t>
   </si>
   <si>
@@ -72,7 +78,7 @@
     <t xml:space="preserve">feed_price</t>
   </si>
   <si>
-    <t xml:space="preserve">misc</t>
+    <t xml:space="preserve">feed_per_pig</t>
   </si>
   <si>
     <t xml:space="preserve">average_age</t>
@@ -112,63 +118,6 @@
   </si>
   <si>
     <t xml:space="preserve">dec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feed Mass (Kg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feed Price (E)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Misc (E)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Age (Days)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feed per Pig (Kg/pig)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feed per Age per Pig (Kg/[Day/Pig])</t>
   </si>
 </sst>
 </file>
@@ -260,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -282,6 +231,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,14 +270,14 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.43"/>
   </cols>
@@ -357,10 +310,15 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -385,10 +343,16 @@
         <v>2100</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>44141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -414,10 +378,16 @@
         <v>2700</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>44275</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -443,10 +413,16 @@
         <v>2800</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>44275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -472,10 +448,16 @@
         <v>2088</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>44352</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -501,10 +483,16 @@
         <v>2340</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>44352</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -519,10 +507,16 @@
       </c>
       <c r="D7" s="5"/>
       <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>44427</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -537,10 +531,16 @@
       </c>
       <c r="D8" s="5"/>
       <c r="H8" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>40</v>
+        <v>10</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>44427</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -554,11 +554,18 @@
         <v>500</v>
       </c>
       <c r="D9" s="5"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>44427</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -572,14 +579,28 @@
         <v>500</v>
       </c>
       <c r="D10" s="5"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>40</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>44427</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="K11" s="5"/>
+    </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -677,37 +698,37 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>12</v>
+      <c r="A1" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -727,7 +748,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -747,7 +768,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
@@ -767,7 +788,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
@@ -787,7 +808,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3</v>
@@ -799,16 +820,16 @@
         <v>960</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="J6" s="7"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>3</v>
@@ -820,7 +841,7 @@
         <v>624</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>77</v>
@@ -830,7 +851,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -842,49 +863,49 @@
         <v>1292</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>54.8114219097222</v>
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>71</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0</v>
+        <v>1606</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7" t="n">
-        <v>54.8120143055556</v>
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>937</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>56</v>
@@ -892,7 +913,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>4</v>
@@ -903,14 +924,12 @@
       <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0</v>
@@ -921,14 +940,12 @@
       <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0</v>
@@ -939,9 +956,7 @@
       <c r="D13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
   </sheetData>
@@ -960,62 +975,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -1032,31 +1033,17 @@
       <c r="F2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -1073,31 +1060,17 @@
       <c r="F3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
@@ -1114,31 +1087,17 @@
       <c r="F4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
@@ -1155,67 +1114,165 @@
       <c r="F5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>960</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>50</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>624</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>0</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1292</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>0</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Feed eaten by pig is update monthly.
</commit_message>
<xml_diff>
--- a/Files/spread.xlsx
+++ b/Files/spread.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -63,10 +63,22 @@
     <t xml:space="preserve">n</t>
   </si>
   <si>
+    <t xml:space="preserve">1.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">m</t>
   </si>
   <si>
+    <t xml:space="preserve">3.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0</t>
   </si>
   <si>
     <t xml:space="preserve">month</t>
@@ -212,7 +224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +246,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,17 +285,17 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -348,8 +364,8 @@
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <v>10</v>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>115</v>
@@ -384,10 +400,10 @@
         <v>2700</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>110</v>
@@ -422,10 +438,10 @@
         <v>2800</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>110</v>
@@ -460,10 +476,10 @@
         <v>2088</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>108</v>
@@ -498,10 +514,10 @@
         <v>2340</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>108</v>
@@ -538,8 +554,8 @@
       <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="1" t="n">
-        <v>10</v>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>62.5</v>
@@ -570,14 +586,14 @@
       <c r="F8" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>1560</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="1" t="n">
-        <v>10</v>
+      <c r="I8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="J8" s="1" t="n">
         <v>62.5</v>
@@ -604,11 +620,11 @@
       <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>0</v>
+      <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>62.5</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>44427</v>
@@ -632,11 +648,11 @@
       <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <v>0</v>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>62.5</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>44427</v>
@@ -748,37 +764,37 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
+      <c r="A1" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -798,7 +814,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -818,7 +834,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
@@ -838,7 +854,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
@@ -858,7 +874,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3</v>
@@ -875,11 +891,11 @@
       <c r="F6" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="J6" s="7"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>3</v>
@@ -901,7 +917,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -923,7 +939,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>6</v>
@@ -943,7 +959,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>4</v>
@@ -963,7 +979,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>2</v>
@@ -975,15 +991,15 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>0</v>
+        <v>62.5</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>2</v>
@@ -1003,7 +1019,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0</v>
@@ -1043,30 +1059,30 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
+      <c r="A1" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1078,7 +1094,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -1105,7 +1121,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -1132,7 +1148,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
@@ -1159,7 +1175,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
@@ -1186,7 +1202,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3</v>
@@ -1204,11 +1220,11 @@
         <v>96</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="8"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>3</v>
@@ -1230,7 +1246,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>6</v>
@@ -1252,7 +1268,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>6</v>
@@ -1270,7 +1286,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>4</v>
@@ -1290,7 +1306,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>4</v>
@@ -1306,7 +1322,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0</v>
@@ -1322,7 +1338,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0</v>

</xml_diff>